<commit_message>
finish tests for schedule and addresses
</commit_message>
<xml_diff>
--- a/test/groups2.xlsx
+++ b/test/groups2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gperry\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFD4FB0-6397-45A5-824E-909AF39DFAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A5FEB1-4247-4DCD-9F9E-D38B9959F50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet 1 - 2023-fall-small-group" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1 - 2023-fall-small-group'!$A$1:$AA$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1 - 2023-fall-small-group'!$A$1:$AA$14</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="235">
   <si>
     <t>Submission ID</t>
   </si>
@@ -241,9 +241,6 @@
     <t>Thursday</t>
   </si>
   <si>
-    <t>6 pm</t>
-  </si>
-  <si>
     <t>Michelle</t>
   </si>
   <si>
@@ -532,18 +529,7 @@
     </r>
   </si>
   <si>
-    <t>2023-08-21 12:55:18 pm</t>
-  </si>
-  <si>
     <t>Mobile: (256) 698-9762</t>
-  </si>
-  <si>
-    <t>Home:
-412 White Petal Street SW
-Huntsville , Al 35824</t>
-  </si>
-  <si>
-    <t>Debbie Mathis</t>
   </si>
   <si>
     <r>
@@ -557,19 +543,7 @@
     </r>
   </si>
   <si>
-    <t>A Study of the Book of Habakkuk</t>
-  </si>
-  <si>
-    <t>This Small Group will be using the Book Embracing Joy. By Jean Wilund. For an in depth study of the Book of Habakkuk. We will also watch some short videos about this Minor Prophet Book.</t>
-  </si>
-  <si>
-    <t>Cindy and Roger Tadsen’s house at 109 Hidden Creek Dr. Huntsville Al 35806</t>
-  </si>
-  <si>
     <t>3:30 - 5:00</t>
-  </si>
-  <si>
-    <t>Bible Study, Book Study</t>
   </si>
   <si>
     <t>2023-08-21 1:04:39 pm</t>
@@ -2307,10 +2281,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA18"/>
+  <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -2503,7 +2477,7 @@
         <v>65</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>45</v>
@@ -2517,31 +2491,31 @@
         <v>17451240</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="F3" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>57</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>28</v>
@@ -2551,10 +2525,10 @@
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>39</v>
@@ -2563,7 +2537,7 @@
         <v>35</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U3" s="8"/>
       <c r="V3" s="5" t="s">
@@ -2573,13 +2547,13 @@
         <v>40</v>
       </c>
       <c r="X3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y3" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="Z3" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="AA3" s="5" t="s">
         <v>30</v>
@@ -2590,25 +2564,25 @@
         <v>17555705</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="F4" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>57</v>
@@ -2620,28 +2594,28 @@
         <v>43</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
       <c r="P4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q4" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T4" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="U4" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>30</v>
@@ -2650,13 +2624,13 @@
         <v>40</v>
       </c>
       <c r="X4" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y4" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="Y4" s="5" t="s">
+      <c r="Z4" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="Z4" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="AA4" s="5" t="s">
         <v>30</v>
@@ -2667,28 +2641,28 @@
         <v>17569378</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="F5" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="I5" s="5" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>38</v>
@@ -2697,10 +2671,10 @@
         <v>43</v>
       </c>
       <c r="L5" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="N5" s="6">
         <v>2566517687</v>
@@ -2709,10 +2683,10 @@
         <v>42</v>
       </c>
       <c r="P5" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q5" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>34</v>
@@ -2737,7 +2711,7 @@
         <v>108</v>
       </c>
       <c r="Z5" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AA5" s="5" t="s">
         <v>33</v>
@@ -2748,25 +2722,25 @@
         <v>17632291</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="F6" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>57</v>
@@ -2778,13 +2752,13 @@
         <v>43</v>
       </c>
       <c r="L6" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="O6" s="5" t="s">
         <v>47</v>
@@ -2793,7 +2767,7 @@
         <v>45</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>34</v>
@@ -2815,7 +2789,7 @@
         <v>32</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z6" s="5" t="s">
         <v>45</v>
@@ -2829,31 +2803,31 @@
         <v>17699180</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>127</v>
       </c>
       <c r="F7" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>129</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>57</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>28</v>
@@ -2863,22 +2837,22 @@
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
       <c r="P7" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q7" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="Q7" s="5" t="s">
-        <v>131</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>34</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T7" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="U7" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="U7" s="5" t="s">
-        <v>133</v>
       </c>
       <c r="V7" s="5" t="s">
         <v>30</v>
@@ -2887,13 +2861,13 @@
         <v>40</v>
       </c>
       <c r="X7" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y7" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="Y7" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="Z7" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA7" s="5" t="s">
         <v>33</v>
@@ -2901,28 +2875,28 @@
     </row>
     <row r="8" spans="1:27" ht="36" customHeight="1">
       <c r="A8" s="3">
-        <v>17719275</v>
+        <v>17719501</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>139</v>
-      </c>
       <c r="H8" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>57</v>
@@ -2934,10 +2908,10 @@
         <v>43</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="N8" s="6">
         <v>2566583040</v>
@@ -2973,78 +2947,78 @@
         <v>41</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>147</v>
+        <v>80</v>
       </c>
       <c r="AA8" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="36" customHeight="1">
+    <row r="9" spans="1:27" ht="44.1" customHeight="1">
       <c r="A9" s="3">
-        <v>17719501</v>
+        <v>17722818</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F9" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>57</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>43</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="N9" s="6">
-        <v>2566583040</v>
+        <v>2564546909</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="T9" s="5" t="s">
         <v>46</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="V9" s="5" t="s">
         <v>30</v>
@@ -3053,13 +3027,13 @@
         <v>40</v>
       </c>
       <c r="X9" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="Y9" s="5" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="Z9" s="5" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="AA9" s="5" t="s">
         <v>33</v>
@@ -3067,67 +3041,67 @@
     </row>
     <row r="10" spans="1:27" ht="44.1" customHeight="1">
       <c r="A10" s="3">
-        <v>17722818</v>
+        <v>17724112</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="F10" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>57</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>43</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="N10" s="6">
-        <v>2564546909</v>
+        <v>12566056652</v>
       </c>
       <c r="O10" s="5" t="s">
         <v>38</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="T10" s="5" t="s">
         <v>46</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="V10" s="5" t="s">
         <v>30</v>
@@ -3136,13 +3110,13 @@
         <v>40</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="Y10" s="5" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="Z10" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AA10" s="5" t="s">
         <v>33</v>
@@ -3150,58 +3124,58 @@
     </row>
     <row r="11" spans="1:27" ht="44.1" customHeight="1">
       <c r="A11" s="3">
-        <v>17724112</v>
+        <v>17738762</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F11" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>57</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>43</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="N11" s="6">
-        <v>12566056652</v>
+        <v>177</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>178</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>38</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="S11" s="5" t="s">
         <v>29</v>
@@ -3210,105 +3184,101 @@
         <v>46</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="W11" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="X11" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Y11" s="5" t="s">
-        <v>177</v>
+        <v>108</v>
       </c>
       <c r="Z11" s="5" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="AA11" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="44.1" customHeight="1">
+    <row r="12" spans="1:27" ht="51" customHeight="1">
       <c r="A12" s="3">
-        <v>17738762</v>
+        <v>17745592</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F12" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>57</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>43</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="M12" s="8"/>
+      <c r="N12" s="6">
+        <v>9124295306</v>
+      </c>
+      <c r="O12" s="8"/>
       <c r="P12" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="S12" s="5" t="s">
         <v>29</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>46</v>
+        <v>190</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="W12" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="Y12" s="5" t="s">
-        <v>109</v>
+        <v>192</v>
       </c>
       <c r="Z12" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA12" s="5" t="s">
         <v>33</v>
@@ -3316,262 +3286,251 @@
     </row>
     <row r="13" spans="1:27" ht="51" customHeight="1">
       <c r="A13" s="3">
-        <v>17745592</v>
+        <v>17794950</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="F13" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>57</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>43</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="M13" s="8"/>
-      <c r="N13" s="6">
-        <v>9124295306</v>
-      </c>
-      <c r="O13" s="8"/>
+        <v>200</v>
+      </c>
+      <c r="M13" s="10"/>
+      <c r="N13" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="P13" s="5" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="R13" s="5" t="s">
         <v>34</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="T13" s="5" t="s">
-        <v>198</v>
+        <v>46</v>
       </c>
       <c r="U13" s="5" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="V13" s="5" t="s">
         <v>30</v>
       </c>
       <c r="W13" s="5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="X13" s="5" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="Y13" s="5" t="s">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="Z13" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AA13" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="51" customHeight="1">
+    <row r="14" spans="1:27" ht="46.5" customHeight="1">
       <c r="A14" s="3">
-        <v>17794950</v>
+        <v>17850822</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F14" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>57</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>43</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="M14" s="10"/>
-      <c r="N14" s="5" t="s">
-        <v>209</v>
+        <v>211</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="N14" s="6">
+        <v>2544664501</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="R14" s="5" t="s">
         <v>34</v>
       </c>
       <c r="S14" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="T14" s="5" t="s">
         <v>46</v>
       </c>
       <c r="U14" s="5" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="V14" s="5" t="s">
         <v>30</v>
       </c>
       <c r="W14" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="X14" s="5" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="Y14" s="5" t="s">
-        <v>50</v>
+        <v>216</v>
       </c>
       <c r="Z14" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AA14" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="46.5" customHeight="1">
-      <c r="A15" s="3">
-        <v>17850822</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="F15" s="6" t="b">
-        <v>1</v>
+    <row r="15" spans="1:27" ht="102.75" customHeight="1">
+      <c r="B15" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>217</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="I15" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="M15" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="N15" s="6">
-        <v>2544664501</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P15" s="5" t="s">
+      <c r="N15" s="10" t="s">
         <v>221</v>
       </c>
+      <c r="P15" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="Q15" s="5" t="s">
-        <v>222</v>
+        <v>61</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="T15" s="5" t="s">
         <v>46</v>
       </c>
       <c r="U15" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="V15" s="5" t="s">
-        <v>30</v>
+        <v>215</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="W15" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="Y15" s="5" t="s">
-        <v>224</v>
+        <v>111</v>
       </c>
       <c r="Z15" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA15" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="102.75" customHeight="1">
+    <row r="16" spans="1:27" ht="19.899999999999999" customHeight="1">
       <c r="B16" s="1" t="s">
-        <v>219</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>218</v>
+        <v>222</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>229</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>57</v>
@@ -3580,13 +3539,13 @@
         <v>43</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="M16" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="N16" s="10" t="s">
-        <v>229</v>
+        <v>223</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>45</v>
@@ -3598,25 +3557,25 @@
         <v>39</v>
       </c>
       <c r="S16" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="U16" s="5" t="s">
-        <v>223</v>
+      <c r="U16" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="W16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="X16" s="5" t="s">
-        <v>32</v>
+      <c r="X16" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="Y16" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Z16" s="5" t="s">
         <v>45</v>
@@ -3627,52 +3586,40 @@
     </row>
     <row r="17" spans="2:27" ht="19.899999999999999" customHeight="1">
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>211</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>237</v>
+        <v>206</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>210</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>57</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q17" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="M17" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="N17" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q17" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="R17" s="5" t="s">
         <v>39</v>
       </c>
       <c r="S17" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="T17" s="5" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="V17" s="1" t="s">
         <v>30</v>
@@ -3681,76 +3628,20 @@
         <v>40</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y17" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z17" s="5" t="s">
-        <v>45</v>
+        <v>76</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="AA17" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="2:27" ht="19.899999999999999" customHeight="1">
-      <c r="B18" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="R18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="S18" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="X18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y18" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="Z18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA18" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:AA15" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:AA14" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="8">
       <filters>
         <filter val="Cullman, Hartselle, Madison"/>
@@ -3767,28 +3658,26 @@
     <hyperlink ref="D6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
     <hyperlink ref="M6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
     <hyperlink ref="D7" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="D8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="M8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="D9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="M9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="D10" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="M10" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="D11" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="M11" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="D12" r:id="rId17" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="M12" r:id="rId18" display="kupono09@gmail.com" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="D13" r:id="rId19" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="D14" r:id="rId20" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="D15" r:id="rId21" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="M15" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="D16" r:id="rId23" xr:uid="{604B3EC2-08CC-4D41-A466-329DFC3C28CC}"/>
-    <hyperlink ref="N17" r:id="rId24" display="tel:(256) 735-9831" xr:uid="{C17B87A8-360A-4124-87B9-20C6B56493BD}"/>
-    <hyperlink ref="M17" r:id="rId25" display="garrettmanley13@yahoo.com //" xr:uid="{BD1E57FF-7715-4D0E-8582-A920E1BE49AC}"/>
-    <hyperlink ref="D18" r:id="rId26" xr:uid="{EB51886D-41A3-4C6C-B0C5-96345EFC63CA}"/>
-    <hyperlink ref="D4" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="D9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="M9" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="D10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="M10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="D11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="M11" r:id="rId14" display="kupono09@gmail.com" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="D12" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="D13" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="D14" r:id="rId17" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="M14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="D15" r:id="rId19" xr:uid="{604B3EC2-08CC-4D41-A466-329DFC3C28CC}"/>
+    <hyperlink ref="N16" r:id="rId20" display="tel:(256) 735-9831" xr:uid="{C17B87A8-360A-4124-87B9-20C6B56493BD}"/>
+    <hyperlink ref="M16" r:id="rId21" display="garrettmanley13@yahoo.com //" xr:uid="{BD1E57FF-7715-4D0E-8582-A920E1BE49AC}"/>
+    <hyperlink ref="D17" r:id="rId22" xr:uid="{EB51886D-41A3-4C6C-B0C5-96345EFC63CA}"/>
+    <hyperlink ref="D4" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="M8" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="D8" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>